<commit_message>
Fixed IAM Test cases.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
   <si>
     <t>TCID</t>
   </si>
@@ -65,31 +65,13 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>amneetsingh50@gmail.com</t>
-  </si>
-  <si>
     <t>Transaction@2</t>
   </si>
   <si>
-    <t>amneetsingh500@gmail.com</t>
-  </si>
-  <si>
     <t>transaction@2</t>
   </si>
   <si>
     <t>EMAIL</t>
-  </si>
-  <si>
-    <t>amneetsingh100@gmail.com</t>
-  </si>
-  <si>
-    <t>amneetsingh10@gmail.com</t>
-  </si>
-  <si>
-    <t>amneet.singh@thomsonreuters.com</t>
-  </si>
-  <si>
-    <t>amneetsingh@thomsonreuters.com</t>
   </si>
   <si>
     <t>SUFFIX</t>
@@ -389,6 +371,39 @@
   </si>
   <si>
     <t>IAM025</t>
+  </si>
+  <si>
+    <t>user1testautomation@gmail.com</t>
+  </si>
+  <si>
+    <t>Neon@123</t>
+  </si>
+  <si>
+    <t>user1testautomatio@gmail.com</t>
+  </si>
+  <si>
+    <t>neonsteamid@gmail.com</t>
+  </si>
+  <si>
+    <t>neon@123</t>
+  </si>
+  <si>
+    <t>neonfbook@gmail.com</t>
+  </si>
+  <si>
+    <t>1Pproject</t>
+  </si>
+  <si>
+    <t>neonfbok@gmail.com</t>
+  </si>
+  <si>
+    <t>1pproject</t>
+  </si>
+  <si>
+    <t>linkedinloginid@gmail.com</t>
+  </si>
+  <si>
+    <t>linkedinlogind@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -476,7 +491,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -500,6 +515,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,17 +823,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -817,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -831,64 +855,64 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -899,13 +923,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -916,13 +940,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -933,13 +957,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -950,13 +974,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -967,13 +991,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -983,48 +1007,48 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="A11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="A12" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1035,13 +1059,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1052,13 +1076,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1069,13 +1093,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1086,13 +1110,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1103,13 +1127,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>5</v>
@@ -1120,13 +1144,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>5</v>
@@ -1135,15 +1159,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="90">
+    <row r="20" spans="1:5" ht="86.4">
       <c r="A20" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1154,13 +1178,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1171,13 +1195,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1186,15 +1210,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5">
       <c r="A23" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1205,13 +1229,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1222,13 +1246,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1239,13 +1263,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
@@ -1268,15 +1292,15 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1287,7 +1311,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1298,7 +1322,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1309,7 +1333,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1320,7 +1344,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1331,7 +1355,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1358,12 +1382,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" width="12.109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.44140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1402,13 +1426,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1427,7 +1451,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -1441,7 +1465,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -1455,7 +1479,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>9</v>
@@ -1478,13 +1502,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1503,7 +1527,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -1517,7 +1541,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -1531,7 +1555,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>9</v>
@@ -1550,22 +1574,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -1579,10 +1603,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1593,10 +1617,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1607,10 +1631,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1631,7 +1655,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1644,7 +1668,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1652,17 +1676,15 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A6" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1673,19 +1695,19 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -1699,10 +1721,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1713,10 +1735,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1727,10 +1749,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1751,7 +1773,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1764,7 +1786,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1775,14 +1797,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A6" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1793,19 +1810,19 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -1819,10 +1836,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1833,10 +1850,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1847,10 +1864,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1871,10 +1888,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1884,9 +1901,9 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1895,14 +1912,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B3:B4" r:id="rId3" display="Neon@123"/>
     <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A6" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1916,12 +1931,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1929,10 +1944,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -1949,7 +1964,7 @@
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
@@ -1967,7 +1982,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
@@ -1985,10 +2000,10 @@
         <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
@@ -2006,7 +2021,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
@@ -2023,7 +2038,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -2055,11 +2070,11 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2078,7 +2093,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>9</v>
@@ -2092,7 +2107,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -2123,13 +2138,13 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2137,10 +2152,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2154,10 +2169,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2169,15 +2184,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2194,10 +2209,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -2214,10 +2229,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -2234,10 +2249,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed IAM Test Scripts.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="124">
   <si>
     <t>TCID</t>
   </si>
@@ -95,25 +95,10 @@
     <t>TICK MARKS</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Weak</t>
   </si>
   <si>
-    <t>Tr</t>
-  </si>
-  <si>
-    <t>Tra</t>
-  </si>
-  <si>
     <t>Good</t>
-  </si>
-  <si>
-    <t>Transact</t>
-  </si>
-  <si>
-    <t>Transact2</t>
   </si>
   <si>
     <t>Strong</t>
@@ -404,6 +389,18 @@
   </si>
   <si>
     <t>linkedinlogind@gmail.com</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>Neo3</t>
+  </si>
+  <si>
+    <t>Neon@</t>
   </si>
 </sst>
 </file>
@@ -823,15 +820,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.77734375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -841,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -855,64 +852,64 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -923,13 +920,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -940,13 +937,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -955,15 +952,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -972,15 +969,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -989,15 +986,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -1008,15 +1005,15 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="16" t="s">
@@ -1025,15 +1022,15 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -1042,13 +1039,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1059,13 +1056,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1074,15 +1071,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1091,15 +1088,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1108,15 +1105,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1127,13 +1124,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>5</v>
@@ -1144,13 +1141,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>5</v>
@@ -1159,15 +1156,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="86.4">
+    <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1178,13 +1175,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1195,13 +1192,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1210,15 +1207,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1229,13 +1226,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1246,13 +1243,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1263,13 +1260,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
@@ -1300,7 +1297,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1311,7 +1308,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1322,7 +1319,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1333,7 +1330,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1344,7 +1341,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1355,7 +1352,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1603,10 +1600,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1617,10 +1614,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1631,10 +1628,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1655,7 +1652,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1668,7 +1665,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1721,10 +1718,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1735,10 +1732,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1749,10 +1746,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1773,7 +1770,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1786,7 +1783,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1836,10 +1833,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1850,10 +1847,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1864,10 +1861,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1888,7 +1885,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1901,7 +1898,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -2135,7 +2132,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2169,10 +2166,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2184,15 +2181,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2209,10 +2206,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -2228,11 +2225,11 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
+      <c r="A5" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -2248,11 +2245,11 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
+      <c r="A6" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -2268,6 +2265,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed failing scripts in IAM and Notification Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>ERROR TEXT</t>
   </si>
   <si>
-    <t>Please enter no more than 70 characters.</t>
-  </si>
-  <si>
     <t>Please enter a valid Email Address.</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>Neon@</t>
+  </si>
+  <si>
+    <t>Please enter no more than 255 characters.</t>
   </si>
 </sst>
 </file>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -852,64 +852,64 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -920,13 +920,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -937,13 +937,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -954,13 +954,13 @@
     </row>
     <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -988,13 +988,13 @@
     </row>
     <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -1005,13 +1005,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
@@ -1022,13 +1022,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>5</v>
@@ -1039,13 +1039,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1090,13 +1090,13 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1107,13 +1107,13 @@
     </row>
     <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1124,13 +1124,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>5</v>
@@ -1141,13 +1141,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>5</v>
@@ -1158,13 +1158,13 @@
     </row>
     <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1175,13 +1175,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1192,13 +1192,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1226,13 +1226,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1243,13 +1243,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1260,13 +1260,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
@@ -1297,7 +1297,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1600,10 +1600,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1628,10 +1628,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1665,7 +1665,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1732,10 +1732,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1783,7 +1783,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1833,10 +1833,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1861,10 +1861,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1898,7 +1898,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7">
-        <v>61</v>
+        <v>246</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7">
-        <v>62</v>
+        <v>247</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>17</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7">
-        <v>63</v>
+        <v>248</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
@@ -2149,10 +2149,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2181,15 +2181,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2206,10 +2206,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -2226,10 +2226,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed 3 watchlist test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>ERROR TEXT</t>
   </si>
   <si>
-    <t>Please enter no more than 70 characters.</t>
-  </si>
-  <si>
     <t>Please enter a valid Email Address.</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>Neon@</t>
+  </si>
+  <si>
+    <t>Please enter no more than 255 characters.</t>
   </si>
 </sst>
 </file>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -852,64 +852,64 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -920,13 +920,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -937,13 +937,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -954,13 +954,13 @@
     </row>
     <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -988,13 +988,13 @@
     </row>
     <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -1005,13 +1005,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
@@ -1022,13 +1022,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>5</v>
@@ -1039,13 +1039,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1090,13 +1090,13 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1107,13 +1107,13 @@
     </row>
     <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1124,13 +1124,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>5</v>
@@ -1141,13 +1141,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>5</v>
@@ -1158,13 +1158,13 @@
     </row>
     <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1175,13 +1175,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1192,13 +1192,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1226,13 +1226,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1243,13 +1243,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1260,13 +1260,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
@@ -1297,7 +1297,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1600,10 +1600,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1628,10 +1628,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1665,7 +1665,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1732,10 +1732,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1783,7 +1783,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1833,10 +1833,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1861,10 +1861,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1898,7 +1898,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7">
-        <v>61</v>
+        <v>246</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7">
-        <v>62</v>
+        <v>247</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>17</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7">
-        <v>63</v>
+        <v>248</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
@@ -2149,10 +2149,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2181,15 +2181,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2206,10 +2206,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -2226,10 +2226,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed test scripts in IAM
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,289 @@
     <t>Verify that Linkedin CANCEL button is working correctly</t>
   </si>
   <si>
-    <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new TR user registration page:
+    <t>Special character</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
+  </si>
+  <si>
+    <t>Jira id</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login with existing LI id and logout successfully</t>
+  </si>
+  <si>
+    <t>Verify that existing FB user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using FB option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using LI option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify CONFIRM PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
+  </si>
+  <si>
+    <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
+  </si>
+  <si>
+    <t>OPQA-205</t>
+  </si>
+  <si>
+    <t>OPQA-335</t>
+  </si>
+  <si>
+    <t>OPQA-346</t>
+  </si>
+  <si>
+    <t>OPQA-350</t>
+  </si>
+  <si>
+    <t>OPQA-391</t>
+  </si>
+  <si>
+    <t>OPQA-393</t>
+  </si>
+  <si>
+    <t>OPQA-353</t>
+  </si>
+  <si>
+    <t>OPQA-355</t>
+  </si>
+  <si>
+    <t>OPQA-356</t>
+  </si>
+  <si>
+    <t>OPQA-357</t>
+  </si>
+  <si>
+    <t>OPQA-395</t>
+  </si>
+  <si>
+    <t>OPQA-394</t>
+  </si>
+  <si>
+    <t>OPQA-397</t>
+  </si>
+  <si>
+    <t>OPQA-400</t>
+  </si>
+  <si>
+    <t>OPQA-523</t>
+  </si>
+  <si>
+    <t>OPQA-535</t>
+  </si>
+  <si>
+    <t>OPQA-538</t>
+  </si>
+  <si>
+    <t>OPQA-724</t>
+  </si>
+  <si>
+    <t>OPQA-725</t>
+  </si>
+  <si>
+    <t>OPQA-551</t>
+  </si>
+  <si>
+    <t>Verify View additional email preferences link is working</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.</t>
+  </si>
+  <si>
+    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
+  </si>
+  <si>
+    <t>OPQA-854,OPQA-853</t>
+  </si>
+  <si>
+    <t>OPQA-399</t>
+  </si>
+  <si>
+    <t>OPQA-527</t>
+  </si>
+  <si>
+    <t>OPQA-525</t>
+  </si>
+  <si>
+    <t>OPQA-529</t>
+  </si>
+  <si>
+    <t>Verify that Help link is working properly</t>
+  </si>
+  <si>
+    <t>IAM001</t>
+  </si>
+  <si>
+    <t>IAM002</t>
+  </si>
+  <si>
+    <t>IAM003</t>
+  </si>
+  <si>
+    <t>IAM004</t>
+  </si>
+  <si>
+    <t>IAM005</t>
+  </si>
+  <si>
+    <t>IAM006</t>
+  </si>
+  <si>
+    <t>IAM007</t>
+  </si>
+  <si>
+    <t>IAM008</t>
+  </si>
+  <si>
+    <t>IAM009</t>
+  </si>
+  <si>
+    <t>IAM010</t>
+  </si>
+  <si>
+    <t>IAM011</t>
+  </si>
+  <si>
+    <t>IAM012</t>
+  </si>
+  <si>
+    <t>IAM019</t>
+  </si>
+  <si>
+    <t>IAM013</t>
+  </si>
+  <si>
+    <t>IAM014</t>
+  </si>
+  <si>
+    <t>IAM015</t>
+  </si>
+  <si>
+    <t>IAM016</t>
+  </si>
+  <si>
+    <t>IAM017</t>
+  </si>
+  <si>
+    <t>IAM018</t>
+  </si>
+  <si>
+    <t>IAM020</t>
+  </si>
+  <si>
+    <t>IAM021</t>
+  </si>
+  <si>
+    <t>IAM022</t>
+  </si>
+  <si>
+    <t>IAM023</t>
+  </si>
+  <si>
+    <t>IAM024</t>
+  </si>
+  <si>
+    <t>IAM025</t>
+  </si>
+  <si>
+    <t>user1testautomation@gmail.com</t>
+  </si>
+  <si>
+    <t>Neon@123</t>
+  </si>
+  <si>
+    <t>user1testautomatio@gmail.com</t>
+  </si>
+  <si>
+    <t>neonsteamid@gmail.com</t>
+  </si>
+  <si>
+    <t>neon@123</t>
+  </si>
+  <si>
+    <t>neonfbook@gmail.com</t>
+  </si>
+  <si>
+    <t>1Pproject</t>
+  </si>
+  <si>
+    <t>neonfbok@gmail.com</t>
+  </si>
+  <si>
+    <t>1pproject</t>
+  </si>
+  <si>
+    <t>linkedinloginid@gmail.com</t>
+  </si>
+  <si>
+    <t>linkedinlogind@gmail.com</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>Neo3</t>
+  </si>
+  <si>
+    <t>Neon@</t>
+  </si>
+  <si>
+    <t>Please enter no more than 255 characters.</t>
+  </si>
+  <si>
+    <t>Verify that user is able to register for a new STeAM account and is able to login with that</t>
+  </si>
+  <si>
+    <t>Verify FIRST NAME field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify LAST NAME field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using STeAM option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify EMAIL ADDRESS field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify PASSWORD field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify that sign up button should be disabled to submit Neon user registration form without filling in the required fields</t>
+  </si>
+  <si>
+    <t>Verify that Neon application doesn't allow the user to create a new account with an email id that has already been used</t>
+  </si>
+  <si>
+    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password</t>
+  </si>
+  <si>
+    <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new Neon user registration page:
 1)        *
 2)        (
 3)        )
@@ -118,289 +400,7 @@
 5)        !</t>
   </si>
   <si>
-    <t>Special character</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>(</t>
-  </si>
-  <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t>&amp;</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
-  </si>
-  <si>
-    <t>Jira id</t>
-  </si>
-  <si>
-    <t>Verify that user is able to register for a new TR account and is able to login with that</t>
-  </si>
-  <si>
-    <t>Verify that user is able to login with existing LI id and logout successfully</t>
-  </si>
-  <si>
-    <t>Verify that existing FB user is able to login and logout successfully</t>
-  </si>
-  <si>
-    <t>Verify FIRST NAME field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify LAST NAME field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using FB option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using LI option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using TR option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify EMAIL ADDRESS field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify CONFIRM PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to submit new TR user registration form without filling in the required fields</t>
-  </si>
-  <si>
-    <t>Verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
-  </si>
-  <si>
-    <t>Verify that user is able to change his TR password by using FORGOT YOUR PASSWORD link and that he is able to login with his new password</t>
-  </si>
-  <si>
-    <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
-  </si>
-  <si>
-    <t>OPQA-205</t>
-  </si>
-  <si>
-    <t>OPQA-335</t>
-  </si>
-  <si>
-    <t>OPQA-346</t>
-  </si>
-  <si>
-    <t>OPQA-350</t>
-  </si>
-  <si>
-    <t>OPQA-391</t>
-  </si>
-  <si>
-    <t>OPQA-393</t>
-  </si>
-  <si>
-    <t>OPQA-353</t>
-  </si>
-  <si>
-    <t>OPQA-355</t>
-  </si>
-  <si>
-    <t>OPQA-356</t>
-  </si>
-  <si>
-    <t>OPQA-357</t>
-  </si>
-  <si>
-    <t>OPQA-395</t>
-  </si>
-  <si>
-    <t>OPQA-394</t>
-  </si>
-  <si>
-    <t>OPQA-397</t>
-  </si>
-  <si>
-    <t>OPQA-400</t>
-  </si>
-  <si>
-    <t>OPQA-523</t>
-  </si>
-  <si>
-    <t>OPQA-535</t>
-  </si>
-  <si>
-    <t>OPQA-538</t>
-  </si>
-  <si>
-    <t>OPQA-724</t>
-  </si>
-  <si>
-    <t>OPQA-725</t>
-  </si>
-  <si>
-    <t>OPQA-551</t>
-  </si>
-  <si>
-    <t>Verify View additional email preferences link is working</t>
-  </si>
-  <si>
-    <t>Verify change password link in the account page is working correctly.</t>
-  </si>
-  <si>
-    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
-  </si>
-  <si>
-    <t>OPQA-854,OPQA-853</t>
-  </si>
-  <si>
-    <t>OPQA-399</t>
-  </si>
-  <si>
-    <t>OPQA-527</t>
-  </si>
-  <si>
-    <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
-  </si>
-  <si>
-    <t>OPQA-525</t>
-  </si>
-  <si>
-    <t>OPQA-529</t>
-  </si>
-  <si>
-    <t>Verify that Help link is working properly</t>
-  </si>
-  <si>
-    <t>IAM001</t>
-  </si>
-  <si>
-    <t>IAM002</t>
-  </si>
-  <si>
-    <t>IAM003</t>
-  </si>
-  <si>
-    <t>IAM004</t>
-  </si>
-  <si>
-    <t>IAM005</t>
-  </si>
-  <si>
-    <t>IAM006</t>
-  </si>
-  <si>
-    <t>IAM007</t>
-  </si>
-  <si>
-    <t>IAM008</t>
-  </si>
-  <si>
-    <t>IAM009</t>
-  </si>
-  <si>
-    <t>IAM010</t>
-  </si>
-  <si>
-    <t>IAM011</t>
-  </si>
-  <si>
-    <t>IAM012</t>
-  </si>
-  <si>
-    <t>IAM019</t>
-  </si>
-  <si>
-    <t>IAM013</t>
-  </si>
-  <si>
-    <t>IAM014</t>
-  </si>
-  <si>
-    <t>IAM015</t>
-  </si>
-  <si>
-    <t>IAM016</t>
-  </si>
-  <si>
-    <t>IAM017</t>
-  </si>
-  <si>
-    <t>IAM018</t>
-  </si>
-  <si>
-    <t>IAM020</t>
-  </si>
-  <si>
-    <t>IAM021</t>
-  </si>
-  <si>
-    <t>IAM022</t>
-  </si>
-  <si>
-    <t>IAM023</t>
-  </si>
-  <si>
-    <t>IAM024</t>
-  </si>
-  <si>
-    <t>IAM025</t>
-  </si>
-  <si>
-    <t>user1testautomation@gmail.com</t>
-  </si>
-  <si>
-    <t>Neon@123</t>
-  </si>
-  <si>
-    <t>user1testautomatio@gmail.com</t>
-  </si>
-  <si>
-    <t>neonsteamid@gmail.com</t>
-  </si>
-  <si>
-    <t>neon@123</t>
-  </si>
-  <si>
-    <t>neonfbook@gmail.com</t>
-  </si>
-  <si>
-    <t>1Pproject</t>
-  </si>
-  <si>
-    <t>neonfbok@gmail.com</t>
-  </si>
-  <si>
-    <t>1pproject</t>
-  </si>
-  <si>
-    <t>linkedinloginid@gmail.com</t>
-  </si>
-  <si>
-    <t>linkedinlogind@gmail.com</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Ne</t>
-  </si>
-  <si>
-    <t>Neo3</t>
-  </si>
-  <si>
-    <t>Neon@</t>
-  </si>
-  <si>
-    <t>Please enter no more than 255 characters.</t>
+    <t>Verify that STeAM account gets locked after 10 consecutive unsuccessful login attempts</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -516,9 +516,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -820,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -838,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -850,15 +847,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="28.8">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -869,10 +866,10 @@
     </row>
     <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>26</v>
@@ -886,13 +883,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
@@ -903,13 +900,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -920,13 +917,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -937,13 +934,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -954,13 +951,13 @@
     </row>
     <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -971,13 +968,13 @@
     </row>
     <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="6" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -988,13 +985,13 @@
     </row>
     <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -1005,47 +1002,47 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1056,13 +1053,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1073,13 +1070,13 @@
     </row>
     <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1090,13 +1087,13 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1107,13 +1104,13 @@
     </row>
     <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1124,13 +1121,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>5</v>
@@ -1141,10 +1138,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>27</v>
@@ -1158,13 +1155,13 @@
     </row>
     <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="6" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1175,13 +1172,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1192,13 +1189,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1209,13 +1206,13 @@
     </row>
     <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1226,13 +1223,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1243,13 +1240,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1260,13 +1257,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
@@ -1297,7 +1294,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1308,7 +1305,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1319,7 +1316,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1330,7 +1327,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1341,7 +1338,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1352,7 +1349,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1600,10 +1597,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1614,10 +1611,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1628,10 +1625,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1652,7 +1649,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1665,7 +1662,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1718,10 +1715,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1732,10 +1729,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1746,10 +1743,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1770,7 +1767,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1783,7 +1780,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1833,10 +1830,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1847,10 +1844,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1861,10 +1858,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1885,7 +1882,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1898,7 +1895,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1924,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2000,7 +1997,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
@@ -2166,7 +2163,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -2186,7 +2183,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -2206,7 +2203,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -2226,7 +2223,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Fixed watchlist test cases for FF
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,289 @@
     <t>Verify that Linkedin CANCEL button is working correctly</t>
   </si>
   <si>
-    <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new TR user registration page:
+    <t>Special character</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
+  </si>
+  <si>
+    <t>Jira id</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login with existing LI id and logout successfully</t>
+  </si>
+  <si>
+    <t>Verify that existing FB user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using FB option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using LI option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify CONFIRM PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
+  </si>
+  <si>
+    <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
+  </si>
+  <si>
+    <t>OPQA-205</t>
+  </si>
+  <si>
+    <t>OPQA-335</t>
+  </si>
+  <si>
+    <t>OPQA-346</t>
+  </si>
+  <si>
+    <t>OPQA-350</t>
+  </si>
+  <si>
+    <t>OPQA-391</t>
+  </si>
+  <si>
+    <t>OPQA-393</t>
+  </si>
+  <si>
+    <t>OPQA-353</t>
+  </si>
+  <si>
+    <t>OPQA-355</t>
+  </si>
+  <si>
+    <t>OPQA-356</t>
+  </si>
+  <si>
+    <t>OPQA-357</t>
+  </si>
+  <si>
+    <t>OPQA-395</t>
+  </si>
+  <si>
+    <t>OPQA-394</t>
+  </si>
+  <si>
+    <t>OPQA-397</t>
+  </si>
+  <si>
+    <t>OPQA-400</t>
+  </si>
+  <si>
+    <t>OPQA-523</t>
+  </si>
+  <si>
+    <t>OPQA-535</t>
+  </si>
+  <si>
+    <t>OPQA-538</t>
+  </si>
+  <si>
+    <t>OPQA-724</t>
+  </si>
+  <si>
+    <t>OPQA-725</t>
+  </si>
+  <si>
+    <t>OPQA-551</t>
+  </si>
+  <si>
+    <t>Verify View additional email preferences link is working</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.</t>
+  </si>
+  <si>
+    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
+  </si>
+  <si>
+    <t>OPQA-854,OPQA-853</t>
+  </si>
+  <si>
+    <t>OPQA-399</t>
+  </si>
+  <si>
+    <t>OPQA-527</t>
+  </si>
+  <si>
+    <t>OPQA-525</t>
+  </si>
+  <si>
+    <t>OPQA-529</t>
+  </si>
+  <si>
+    <t>Verify that Help link is working properly</t>
+  </si>
+  <si>
+    <t>IAM001</t>
+  </si>
+  <si>
+    <t>IAM002</t>
+  </si>
+  <si>
+    <t>IAM003</t>
+  </si>
+  <si>
+    <t>IAM004</t>
+  </si>
+  <si>
+    <t>IAM005</t>
+  </si>
+  <si>
+    <t>IAM006</t>
+  </si>
+  <si>
+    <t>IAM007</t>
+  </si>
+  <si>
+    <t>IAM008</t>
+  </si>
+  <si>
+    <t>IAM009</t>
+  </si>
+  <si>
+    <t>IAM010</t>
+  </si>
+  <si>
+    <t>IAM011</t>
+  </si>
+  <si>
+    <t>IAM012</t>
+  </si>
+  <si>
+    <t>IAM019</t>
+  </si>
+  <si>
+    <t>IAM013</t>
+  </si>
+  <si>
+    <t>IAM014</t>
+  </si>
+  <si>
+    <t>IAM015</t>
+  </si>
+  <si>
+    <t>IAM016</t>
+  </si>
+  <si>
+    <t>IAM017</t>
+  </si>
+  <si>
+    <t>IAM018</t>
+  </si>
+  <si>
+    <t>IAM020</t>
+  </si>
+  <si>
+    <t>IAM021</t>
+  </si>
+  <si>
+    <t>IAM022</t>
+  </si>
+  <si>
+    <t>IAM023</t>
+  </si>
+  <si>
+    <t>IAM024</t>
+  </si>
+  <si>
+    <t>IAM025</t>
+  </si>
+  <si>
+    <t>user1testautomation@gmail.com</t>
+  </si>
+  <si>
+    <t>Neon@123</t>
+  </si>
+  <si>
+    <t>user1testautomatio@gmail.com</t>
+  </si>
+  <si>
+    <t>neonsteamid@gmail.com</t>
+  </si>
+  <si>
+    <t>neon@123</t>
+  </si>
+  <si>
+    <t>neonfbook@gmail.com</t>
+  </si>
+  <si>
+    <t>1Pproject</t>
+  </si>
+  <si>
+    <t>neonfbok@gmail.com</t>
+  </si>
+  <si>
+    <t>1pproject</t>
+  </si>
+  <si>
+    <t>linkedinloginid@gmail.com</t>
+  </si>
+  <si>
+    <t>linkedinlogind@gmail.com</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>Neo3</t>
+  </si>
+  <si>
+    <t>Neon@</t>
+  </si>
+  <si>
+    <t>Please enter no more than 255 characters.</t>
+  </si>
+  <si>
+    <t>Verify that user is able to register for a new STeAM account and is able to login with that</t>
+  </si>
+  <si>
+    <t>Verify FIRST NAME field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify LAST NAME field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using STeAM option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify EMAIL ADDRESS field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify PASSWORD field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify that sign up button should be disabled to submit Neon user registration form without filling in the required fields</t>
+  </si>
+  <si>
+    <t>Verify that Neon application doesn't allow the user to create a new account with an email id that has already been used</t>
+  </si>
+  <si>
+    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password</t>
+  </si>
+  <si>
+    <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new Neon user registration page:
 1)        *
 2)        (
 3)        )
@@ -118,289 +400,7 @@
 5)        !</t>
   </si>
   <si>
-    <t>Special character</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>(</t>
-  </si>
-  <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t>&amp;</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
-  </si>
-  <si>
-    <t>Jira id</t>
-  </si>
-  <si>
-    <t>Verify that user is able to register for a new TR account and is able to login with that</t>
-  </si>
-  <si>
-    <t>Verify that user is able to login with existing LI id and logout successfully</t>
-  </si>
-  <si>
-    <t>Verify that existing FB user is able to login and logout successfully</t>
-  </si>
-  <si>
-    <t>Verify FIRST NAME field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify LAST NAME field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using FB option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using LI option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using TR option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify EMAIL ADDRESS field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify CONFIRM PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to submit new TR user registration form without filling in the required fields</t>
-  </si>
-  <si>
-    <t>Verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
-  </si>
-  <si>
-    <t>Verify that user is able to change his TR password by using FORGOT YOUR PASSWORD link and that he is able to login with his new password</t>
-  </si>
-  <si>
-    <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
-  </si>
-  <si>
-    <t>OPQA-205</t>
-  </si>
-  <si>
-    <t>OPQA-335</t>
-  </si>
-  <si>
-    <t>OPQA-346</t>
-  </si>
-  <si>
-    <t>OPQA-350</t>
-  </si>
-  <si>
-    <t>OPQA-391</t>
-  </si>
-  <si>
-    <t>OPQA-393</t>
-  </si>
-  <si>
-    <t>OPQA-353</t>
-  </si>
-  <si>
-    <t>OPQA-355</t>
-  </si>
-  <si>
-    <t>OPQA-356</t>
-  </si>
-  <si>
-    <t>OPQA-357</t>
-  </si>
-  <si>
-    <t>OPQA-395</t>
-  </si>
-  <si>
-    <t>OPQA-394</t>
-  </si>
-  <si>
-    <t>OPQA-397</t>
-  </si>
-  <si>
-    <t>OPQA-400</t>
-  </si>
-  <si>
-    <t>OPQA-523</t>
-  </si>
-  <si>
-    <t>OPQA-535</t>
-  </si>
-  <si>
-    <t>OPQA-538</t>
-  </si>
-  <si>
-    <t>OPQA-724</t>
-  </si>
-  <si>
-    <t>OPQA-725</t>
-  </si>
-  <si>
-    <t>OPQA-551</t>
-  </si>
-  <si>
-    <t>Verify View additional email preferences link is working</t>
-  </si>
-  <si>
-    <t>Verify change password link in the account page is working correctly.</t>
-  </si>
-  <si>
-    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
-  </si>
-  <si>
-    <t>OPQA-854,OPQA-853</t>
-  </si>
-  <si>
-    <t>OPQA-399</t>
-  </si>
-  <si>
-    <t>OPQA-527</t>
-  </si>
-  <si>
-    <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
-  </si>
-  <si>
-    <t>OPQA-525</t>
-  </si>
-  <si>
-    <t>OPQA-529</t>
-  </si>
-  <si>
-    <t>Verify that Help link is working properly</t>
-  </si>
-  <si>
-    <t>IAM001</t>
-  </si>
-  <si>
-    <t>IAM002</t>
-  </si>
-  <si>
-    <t>IAM003</t>
-  </si>
-  <si>
-    <t>IAM004</t>
-  </si>
-  <si>
-    <t>IAM005</t>
-  </si>
-  <si>
-    <t>IAM006</t>
-  </si>
-  <si>
-    <t>IAM007</t>
-  </si>
-  <si>
-    <t>IAM008</t>
-  </si>
-  <si>
-    <t>IAM009</t>
-  </si>
-  <si>
-    <t>IAM010</t>
-  </si>
-  <si>
-    <t>IAM011</t>
-  </si>
-  <si>
-    <t>IAM012</t>
-  </si>
-  <si>
-    <t>IAM019</t>
-  </si>
-  <si>
-    <t>IAM013</t>
-  </si>
-  <si>
-    <t>IAM014</t>
-  </si>
-  <si>
-    <t>IAM015</t>
-  </si>
-  <si>
-    <t>IAM016</t>
-  </si>
-  <si>
-    <t>IAM017</t>
-  </si>
-  <si>
-    <t>IAM018</t>
-  </si>
-  <si>
-    <t>IAM020</t>
-  </si>
-  <si>
-    <t>IAM021</t>
-  </si>
-  <si>
-    <t>IAM022</t>
-  </si>
-  <si>
-    <t>IAM023</t>
-  </si>
-  <si>
-    <t>IAM024</t>
-  </si>
-  <si>
-    <t>IAM025</t>
-  </si>
-  <si>
-    <t>user1testautomation@gmail.com</t>
-  </si>
-  <si>
-    <t>Neon@123</t>
-  </si>
-  <si>
-    <t>user1testautomatio@gmail.com</t>
-  </si>
-  <si>
-    <t>neonsteamid@gmail.com</t>
-  </si>
-  <si>
-    <t>neon@123</t>
-  </si>
-  <si>
-    <t>neonfbook@gmail.com</t>
-  </si>
-  <si>
-    <t>1Pproject</t>
-  </si>
-  <si>
-    <t>neonfbok@gmail.com</t>
-  </si>
-  <si>
-    <t>1pproject</t>
-  </si>
-  <si>
-    <t>linkedinloginid@gmail.com</t>
-  </si>
-  <si>
-    <t>linkedinlogind@gmail.com</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Ne</t>
-  </si>
-  <si>
-    <t>Neo3</t>
-  </si>
-  <si>
-    <t>Neon@</t>
-  </si>
-  <si>
-    <t>Please enter no more than 255 characters.</t>
+    <t>Verify that STeAM account gets locked after 10 consecutive unsuccessful login attempts</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -516,9 +516,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -820,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -838,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -850,15 +847,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="28.8">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -869,10 +866,10 @@
     </row>
     <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>26</v>
@@ -886,13 +883,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
@@ -903,13 +900,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -920,13 +917,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -937,13 +934,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -954,13 +951,13 @@
     </row>
     <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -971,13 +968,13 @@
     </row>
     <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="6" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -988,13 +985,13 @@
     </row>
     <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -1005,47 +1002,47 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1056,13 +1053,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1073,13 +1070,13 @@
     </row>
     <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1090,13 +1087,13 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1107,13 +1104,13 @@
     </row>
     <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1124,13 +1121,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>5</v>
@@ -1141,10 +1138,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>27</v>
@@ -1158,13 +1155,13 @@
     </row>
     <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="6" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1175,13 +1172,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1192,13 +1189,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1209,13 +1206,13 @@
     </row>
     <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1226,13 +1223,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1243,13 +1240,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1260,13 +1257,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
@@ -1297,7 +1294,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1308,7 +1305,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1319,7 +1316,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1330,7 +1327,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1341,7 +1338,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1352,7 +1349,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1600,10 +1597,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1614,10 +1611,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1628,10 +1625,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1652,7 +1649,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1665,7 +1662,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1718,10 +1715,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1732,10 +1729,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1746,10 +1743,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1770,7 +1767,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1783,7 +1780,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1833,10 +1830,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1847,10 +1844,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1861,10 +1858,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1885,7 +1882,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1898,7 +1895,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1924,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2000,7 +1997,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
@@ -2166,7 +2163,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -2186,7 +2183,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -2206,7 +2203,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -2226,7 +2223,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Fixed test scripts in IAM and Notification Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1181,7 +1181,7 @@
         <v>34</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Fixed test scripts in IAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="133">
   <si>
     <t>TCID</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
   </si>
   <si>
-    <t>OPQA-205</t>
-  </si>
-  <si>
     <t>OPQA-335</t>
   </si>
   <si>
@@ -365,22 +362,7 @@
     <t>Please enter no more than 255 characters.</t>
   </si>
   <si>
-    <t>Verify that user is able to register for a new STeAM account and is able to login with that</t>
-  </si>
-  <si>
-    <t>Verify FIRST NAME field in new Neon user registration page</t>
-  </si>
-  <si>
-    <t>Verify LAST NAME field in new Neon user registration page</t>
-  </si>
-  <si>
     <t>Verify that user is not able to login using STeAM option for different negative combinations of username/password</t>
-  </si>
-  <si>
-    <t>Verify EMAIL ADDRESS field in new Neon user registration page</t>
-  </si>
-  <si>
-    <t>Verify PASSWORD field in new Neon user registration page</t>
   </si>
   <si>
     <t>Verify that sign up button should be disabled to submit Neon user registration form without filling in the required fields</t>
@@ -401,6 +383,52 @@
   </si>
   <si>
     <t>Verify that STeAM account gets locked after 10 consecutive unsuccessful login attempts</t>
+  </si>
+  <si>
+    <t>Verify that user is able to register for a new STeAM account and is able to login with that and Verify that user is able to signin using the link in email received after registration</t>
+  </si>
+  <si>
+    <t>OPQA-205,OPQA-531</t>
+  </si>
+  <si>
+    <t>IAM026</t>
+  </si>
+  <si>
+    <t>IAM027</t>
+  </si>
+  <si>
+    <t>OPQA-2794</t>
+  </si>
+  <si>
+    <t>Verify that deep linking is working correctly for account page using STeAM account</t>
+  </si>
+  <si>
+    <t>Verify that deep linking is working correctly for help page using STeAM account</t>
+  </si>
+  <si>
+    <t>OPQA-2795</t>
+  </si>
+  <si>
+    <t>Verify that to validate LAST NAME field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify that to validate FIRST NAME field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify  that to validate EMAIL ADDRESS field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>Verify  that to validate PASSWORD field in new Neon user registration page</t>
+  </si>
+  <si>
+    <t>IAM028</t>
+  </si>
+  <si>
+    <t>OPQA-2905</t>
+  </si>
+  <si>
+    <t>Verify that system able to resend activation mail when user doesn't activated mail and 
+already registered with Neon.</t>
   </si>
 </sst>
 </file>
@@ -815,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -847,15 +875,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8">
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -866,10 +894,10 @@
     </row>
     <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>26</v>
@@ -883,10 +911,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>36</v>
@@ -900,10 +928,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>37</v>
@@ -917,13 +945,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -934,13 +962,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -951,10 +979,10 @@
     </row>
     <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>38</v>
@@ -968,10 +996,10 @@
     </row>
     <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>39</v>
@@ -985,13 +1013,13 @@
     </row>
     <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -1002,13 +1030,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
@@ -1019,16 +1047,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>6</v>
@@ -1036,13 +1064,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1053,10 +1081,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>41</v>
@@ -1070,13 +1098,13 @@
     </row>
     <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1087,13 +1115,13 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1104,13 +1132,13 @@
     </row>
     <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1121,10 +1149,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>42</v>
@@ -1138,10 +1166,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>27</v>
@@ -1155,13 +1183,13 @@
     </row>
     <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1172,16 +1200,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>6</v>
@@ -1189,13 +1217,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1206,13 +1234,13 @@
     </row>
     <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1223,13 +1251,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
@@ -1240,13 +1268,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>5</v>
@@ -1257,18 +1285,69 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="43.2">
+      <c r="A29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1597,10 +1676,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1611,10 +1690,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1625,10 +1704,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1649,7 +1728,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1662,7 +1741,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1715,10 +1794,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1729,10 +1808,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1743,10 +1822,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1767,7 +1846,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1780,7 +1859,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1830,10 +1909,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1844,10 +1923,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1858,10 +1937,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1882,7 +1961,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
@@ -1895,7 +1974,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1997,7 +2076,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
@@ -2163,7 +2242,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -2183,7 +2262,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -2203,7 +2282,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -2223,7 +2302,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -2243,7 +2322,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Taking the latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -17,14 +17,15 @@
     <sheet name="IAM011" sheetId="11" r:id="rId8"/>
     <sheet name="IAM012" sheetId="12" r:id="rId9"/>
     <sheet name="IAM019" sheetId="13" r:id="rId10"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId11"/>
+    <sheet name="IAM029" sheetId="14" r:id="rId11"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="136">
   <si>
     <t>TCID</t>
   </si>
@@ -429,6 +430,15 @@
   <si>
     <t>Verify that system able to resend activation mail when user doesn't activated mail and 
 already registered with Neon.</t>
+  </si>
+  <si>
+    <t>IAM029</t>
+  </si>
+  <si>
+    <t>OPQA-2906</t>
+  </si>
+  <si>
+    <t>Verify that to validate PASSWORD field in new Neon user registration page with maximum length.</t>
   </si>
 </sst>
 </file>
@@ -843,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1348,6 +1358,23 @@
         <v>5</v>
       </c>
       <c r="E29" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8">
+      <c r="A30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1449,6 +1476,77 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>92</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>93</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -1499,7 +1597,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Fixed tests scripts in IAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="142">
   <si>
     <t>TCID</t>
   </si>
@@ -439,6 +439,24 @@
   </si>
   <si>
     <t>Verify that to validate PASSWORD field in new Neon user registration page with maximum length.</t>
+  </si>
+  <si>
+    <t>IAM030</t>
+  </si>
+  <si>
+    <t>IAM031</t>
+  </si>
+  <si>
+    <t>OPQA-2838</t>
+  </si>
+  <si>
+    <t>Verify that deep linking is working correctly for help page using FB and LI accounts</t>
+  </si>
+  <si>
+    <t>OPQA-2837</t>
+  </si>
+  <si>
+    <t>Verify that deep linking is working correctly for account page using FB and LI accounts</t>
   </si>
 </sst>
 </file>
@@ -853,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1375,6 +1393,40 @@
         <v>5</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8">
+      <c r="A31" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified IAM.xlsx and Notification.xlsx files
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,13 @@
     <sheet name="IAM012" sheetId="12" r:id="rId9"/>
     <sheet name="IAM019" sheetId="13" r:id="rId10"/>
     <sheet name="IAM029" sheetId="14" r:id="rId11"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="140">
   <si>
     <t>TCID</t>
   </si>
@@ -34,12 +33,6 @@
   </si>
   <si>
     <t>Runmode</t>
-  </si>
-  <si>
-    <t>TC SCENARIO</t>
-  </si>
-  <si>
-    <t>TC STEPS</t>
   </si>
   <si>
     <t>Y</t>
@@ -463,16 +456,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -539,27 +524,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -570,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -873,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -891,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -900,534 +879,534 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
+        <v>117</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8">
+      <c r="A8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8">
+      <c r="A9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="D9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8">
+      <c r="A10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8">
-      <c r="A8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8">
-      <c r="A9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8">
-      <c r="A10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.8">
+      <c r="A15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8">
+      <c r="A16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8">
+      <c r="A17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="100.8">
+      <c r="A20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8">
+      <c r="A23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="43.2">
+      <c r="A29" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="B29" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8">
-      <c r="A15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28.8">
-      <c r="A16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.8">
-      <c r="A17" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="100.8">
-      <c r="A20" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8">
-      <c r="A23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="43.2">
-      <c r="A29" s="6" t="s">
+      <c r="C29" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8">
+      <c r="A30" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8">
-      <c r="A30" s="6" t="s">
+      <c r="C30" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8">
+      <c r="A31" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8">
-      <c r="A31" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="6" t="s">
+      <c r="C32" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>11</v>
+      <c r="D32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1452,68 +1431,68 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1538,106 +1517,59 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="12.109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.44140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.109375" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="196.5" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="252.75" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1660,58 +1592,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1736,58 +1668,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1812,96 +1744,96 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>104</v>
+      <c r="A4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
-        <v>103</v>
+      <c r="A6" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
-      <c r="B7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
+      <c r="B7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1930,92 +1862,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>104</v>
+      <c r="A4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
-        <v>103</v>
+      <c r="A6" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
-      <c r="B7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
+      <c r="B7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2045,92 +1977,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>97</v>
+      <c r="B4" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
-        <v>98</v>
+      <c r="A6" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
-      <c r="B7" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
+      <c r="B7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2164,78 +2096,78 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>246</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5">
+        <v>247</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7">
-        <v>247</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>248</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2244,34 +2176,34 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2302,44 +2234,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2372,122 +2304,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
-        <v>110</v>
+      <c r="A5" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
-        <v>97</v>
+      <c r="A6" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test cases to IAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="145">
   <si>
     <t>TCID</t>
   </si>
@@ -460,6 +460,14 @@
   <si>
     <t xml:space="preserve">1) Sign-in with Steam and link existing social account with matching email.
 2) Sign-in with Steam account which already has linked social account.
+</t>
+  </si>
+  <si>
+    <t>IAM033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Sign-in with Social and link existing steam  account with matching email.
+2) Sign-in with Social account which already has linked Staem account.
 </t>
   </si>
 </sst>
@@ -540,7 +548,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -564,9 +572,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -864,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:E33"/>
+      <selection activeCell="A33" sqref="A33:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1423,19 +1428,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+    <row r="33" spans="1:5" ht="45">
+      <c r="A33" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
+      <c r="D33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="45">
+      <c r="A34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed scripts in IAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="148">
   <si>
     <t>TCID</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Verify CONFIRM PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
-    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
   </si>
   <si>
     <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
@@ -404,71 +401,83 @@
 </t>
   </si>
   <si>
-    <t>OPQA-356|OPQA-1688</t>
-  </si>
-  <si>
-    <t>Verify that user is not able to login using STeAM option for different negative combinations of username/password|Verify that,user should not able to sign in to Neon,if wrong email address and password is provided.</t>
-  </si>
-  <si>
-    <t>OPQA-335|OPQA-1672|OPQA-1674|OPQA-1929</t>
-  </si>
-  <si>
-    <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process|Verify that user can be able to submit an email address and password(STEAM credentials) on the Neon Landing Screen.|Verify that, user can able to sign in to Neon with STeAM credentials.|Verify that user can able to Sign out from Neon after successful login in "Sign In with Project Neon" in Neon</t>
-  </si>
-  <si>
-    <t>OPQA-350|OPQA-1930</t>
-  </si>
-  <si>
-    <t>Verify that existing FB user is able to login and logout successfully|Verify that user can able to Sign out from Neon after successful login in "Sign In with Facebook" in Neon</t>
-  </si>
-  <si>
-    <t>OPQA-346|OPQA-1931</t>
-  </si>
-  <si>
-    <t>Verify that user is able to login with existing LI id and logout successfully|Verify that user can able to Sign out from Neon after successful login in "Sign In with LinkedIn" in Neon</t>
-  </si>
-  <si>
-    <t>OPQA-2905|OPQA-1841|OPQA-1843|OPQA-1845</t>
+    <t>OPQA-1837||OPQA-1838||OPQA-1844||OPQA-1854||OPQA-1856||OPQA-1857</t>
+  </si>
+  <si>
+    <t>Verify that 'Sign up' link should be displayed on Neon registration page .||Verify that Neon registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email verification Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that After completion of verification process,Neon Identity should be created with steam account.</t>
+  </si>
+  <si>
+    <t>OPQA-2905||OPQA-1841||OPQA-1843|OPQA-1845</t>
   </si>
   <si>
     <t>Verify that system able to resend activation mail when user doesn't activated mail and 
-already registered with Neon.|Verify that,an error message should display as "email activation",when User did'nt activate the link in that respective mail after completing the registration process in Neon.|Verify that, user can click the button to resend email verification,so that the system shall send an email verification to the correct email address,if an email verification message is not sent correctly previously.|Verify that,user should sent to Neon home page after clicking the link in the Neon verification email.</t>
-  </si>
-  <si>
-    <t>OPQA-391|OPQA-1842</t>
-  </si>
-  <si>
-    <t>Verify that to validate FIRST NAME field in new Neon user registration page|Verify that first name and last name should be maximum of 50 characters long and these fields should not be empty.</t>
-  </si>
-  <si>
-    <t>Verify that to validate LAST NAME field in new Neon user registration page|Verify that first name and last name should be maximum of 50 characters long and these fields should not be empty.</t>
-  </si>
-  <si>
-    <t>OPQA-393|OPQA-1842</t>
-  </si>
-  <si>
-    <t>Verify that user is able to register for a new STeAM account and is able to login with that and Verify that user is able to signin using the link in email received after registration|Verify that 'Sign up' link should be displayed on Neon registration page .|Verify that Neon registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).</t>
-  </si>
-  <si>
-    <t>OPQA-205,OPQA-531|OPQA-1837|OPQA-1838</t>
-  </si>
-  <si>
-    <t>Verify  that to validate EMAIL ADDRESS field in new Neon user registration page|Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
-  </si>
-  <si>
-    <t>OPQA-357|OPQA-1839</t>
-  </si>
-  <si>
-    <t>OPQA-394|OPQA-1840</t>
-  </si>
-  <si>
-    <t>Verify  that to validate PASSWORD field in new Neon user registration page|Verify that Passwords should be at least 8 characters,Must contain at least 1 lowercase letter,Must contain at least 1 uppercase letter,Must contain at least 1 number,should have at least one special character and must not be empty.</t>
-  </si>
-  <si>
-    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password|Verify Upon completion of establishing a new password, a user who wants to go to Neon shall be presented a confirmation page with an optional link back to Neon Landing page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPQA-535|OPQA-1955 </t>
+already registered with Neon.||Verify that,an error message should display as "email activation",when User did'nt activate the link in that respective mail after completing the registration process in Neon.||Verify that, user can click the button to resend email verification,so that the system shall send an email verification to the correct email address,if an email verification message is not sent correctly previously.|Verify that,user should sent to Neon home page after clicking the link in the Neon verification email.</t>
+  </si>
+  <si>
+    <t>IAM034</t>
+  </si>
+  <si>
+    <t>Verify that user is able to register for a new STeAM account and is able to login with that|| Verify that user is able to signin using the link in email received after registration</t>
+  </si>
+  <si>
+    <t>OPQA-205||OPQA-531</t>
+  </si>
+  <si>
+    <t>OPQA-335||OPQA-1672||OPQA-1674||OPQA-1929</t>
+  </si>
+  <si>
+    <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process||Verify that user can be able to submit an email address and password(STEAM credentials) on the Neon Landing Screen.||Verify that, user can able to sign in to Neon with STeAM credentials.||Verify that user can able to Sign out from Neon after successful login in "Sign In with Project Neon" in Neon</t>
+  </si>
+  <si>
+    <t>OPQA-346||OPQA-1931</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login with existing LI id and logout successfully||Verify that user can able to Sign out from Neon after successful login in "Sign In with LinkedIn" in Neon</t>
+  </si>
+  <si>
+    <t>OPQA-350||OPQA-1930</t>
+  </si>
+  <si>
+    <t>Verify that existing FB user is able to login and logout successfully||Verify that user can able to Sign out from Neon after successful login in "Sign In with Facebook" in Neon</t>
+  </si>
+  <si>
+    <t>OPQA-391||OPQA-1842</t>
+  </si>
+  <si>
+    <t>Verify that to validate FIRST NAME field in new Neon user registration page||Verify that first name and last name should be maximum of 50 characters long and these fields should not be empty.</t>
+  </si>
+  <si>
+    <t>Verify that to validate LAST NAME field in new Neon user registration page||Verify that first name and last name should be maximum of 50 characters long and these fields should not be empty.</t>
+  </si>
+  <si>
+    <t>OPQA-393||OPQA-1842</t>
+  </si>
+  <si>
+    <t>OPQA-356||OPQA-1688</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using STeAM option for different negative combinations of username/password||Verify that,user should not able to sign in to Neon,if wrong email address and password is provided.</t>
+  </si>
+  <si>
+    <t>Verify  that to validate EMAIL ADDRESS field in new Neon user registration page||Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
+  </si>
+  <si>
+    <t>OPQA-357||OPQA-1839</t>
+  </si>
+  <si>
+    <t>OPQA-394||OPQA-1840</t>
+  </si>
+  <si>
+    <t>Verify  that to validate PASSWORD field in new Neon user registration page||Verify that Passwords should be at least 8 characters,Must contain at least 1 lowercase letter,Must contain at least 1 uppercase letter,Must contain at least 1 number,should have at least one special character and must not be empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQA-535||OPQA-1955 </t>
+  </si>
+  <si>
+    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password||Verify Upon completion of establishing a new password, a user who wants to go to Neon shall be presented a confirmation page with an optional link back to Neon Landing page.</t>
+  </si>
+  <si>
+    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly in Neon and ENW landing page</t>
   </si>
 </sst>
 </file>
@@ -517,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -540,6 +549,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -548,7 +568,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -572,6 +592,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -869,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -901,15 +925,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72">
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -920,13 +944,13 @@
     </row>
     <row r="3" spans="1:5" ht="86.4">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -937,13 +961,13 @@
     </row>
     <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -954,13 +978,13 @@
     </row>
     <row r="5" spans="1:5" ht="43.2">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -971,13 +995,13 @@
     </row>
     <row r="6" spans="1:5" ht="43.2">
       <c r="A6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -988,13 +1012,13 @@
     </row>
     <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
@@ -1005,10 +1029,10 @@
     </row>
     <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>33</v>
@@ -1022,10 +1046,10 @@
     </row>
     <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
@@ -1039,13 +1063,13 @@
     </row>
     <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>3</v>
@@ -1056,13 +1080,13 @@
     </row>
     <row r="11" spans="1:5" ht="43.2">
       <c r="A11" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1073,16 +1097,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>4</v>
@@ -1090,13 +1114,13 @@
     </row>
     <row r="13" spans="1:5" ht="57.6">
       <c r="A13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1105,15 +1129,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1124,13 +1148,13 @@
     </row>
     <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -1141,13 +1165,13 @@
     </row>
     <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3</v>
@@ -1158,13 +1182,13 @@
     </row>
     <row r="17" spans="1:5" ht="57.6">
       <c r="A17" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1175,13 +1199,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -1192,10 +1216,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>24</v>
@@ -1209,13 +1233,13 @@
     </row>
     <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1226,16 +1250,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>4</v>
@@ -1243,13 +1267,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -1260,13 +1284,13 @@
     </row>
     <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -1277,13 +1301,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1294,13 +1318,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>3</v>
@@ -1311,13 +1335,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1328,13 +1352,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1345,13 +1369,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1362,13 +1386,13 @@
     </row>
     <row r="29" spans="1:5" ht="129.6">
       <c r="A29" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1379,13 +1403,13 @@
     </row>
     <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1396,13 +1420,13 @@
     </row>
     <row r="31" spans="1:5" ht="28.8">
       <c r="A31" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>3</v>
@@ -1413,13 +1437,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>3</v>
@@ -1430,13 +1454,13 @@
     </row>
     <row r="33" spans="1:5" ht="43.2">
       <c r="A33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1445,18 +1469,35 @@
     </row>
     <row r="34" spans="1:5" ht="43.2">
       <c r="A34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" ht="129.6">
+      <c r="A35" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2"/>
+      <c r="C35" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,10 +1848,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1821,10 +1862,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1835,10 +1876,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1859,7 +1900,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -1872,7 +1913,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -1925,10 +1966,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1939,10 +1980,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1953,10 +1994,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1977,7 +2018,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -1990,7 +2031,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -2040,10 +2081,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -2054,10 +2095,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -2068,10 +2109,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -2092,7 +2133,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -2105,7 +2146,7 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -2207,7 +2248,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -2373,7 +2414,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -2393,7 +2434,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>20</v>
@@ -2413,7 +2454,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
@@ -2433,7 +2474,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -2453,7 +2494,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Clear unused code in IAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="151">
   <si>
     <t>TCID</t>
   </si>
@@ -471,13 +471,22 @@
     <t>Verify  that to validate PASSWORD field in new Neon user registration page||Verify that Passwords should be at least 8 characters,Must contain at least 1 lowercase letter,Must contain at least 1 uppercase letter,Must contain at least 1 number,should have at least one special character and must not be empty.</t>
   </si>
   <si>
-    <t xml:space="preserve">OPQA-535||OPQA-1955 </t>
-  </si>
-  <si>
-    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password||Verify Upon completion of establishing a new password, a user who wants to go to Neon shall be presented a confirmation page with an optional link back to Neon Landing page.</t>
-  </si>
-  <si>
     <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly in Neon and ENW landing page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password||Verify Upon completion of establishing a new password, a user who wants to go to Neon shall be presented a confirmation page with an optional link back to Neon Landing page.||Verify that,the system should support a Neon password reset workflow with the following configurations:</t>
+  </si>
+  <si>
+    <t>OPQA-535||OPQA-1955||OPQA-3686</t>
+  </si>
+  <si>
+    <t>IAM035</t>
+  </si>
+  <si>
+    <t>OPQA-1851</t>
+  </si>
+  <si>
+    <t>Verify that system should remove any leading or trailing spaces of an email address entered by the user before validating it.</t>
   </si>
 </sst>
 </file>
@@ -893,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1137,7 +1146,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1180,12 +1189,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="57.6">
+    <row r="17" spans="1:5" ht="86.4">
       <c r="A17" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>146</v>
@@ -1496,6 +1505,23 @@
         <v>3</v>
       </c>
       <c r="E35" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8">
+      <c r="A36" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1510,7 +1536,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
New Scripts are added in IAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="157">
   <si>
     <t>TCID</t>
   </si>
@@ -435,12 +435,6 @@
     <t>Verify that user is able to login with existing LI id and logout successfully||Verify that user can able to Sign out from Neon after successful login in "Sign In with LinkedIn" in Neon</t>
   </si>
   <si>
-    <t>OPQA-350||OPQA-1930</t>
-  </si>
-  <si>
-    <t>Verify that existing FB user is able to login and logout successfully||Verify that user can able to Sign out from Neon after successful login in "Sign In with Facebook" in Neon</t>
-  </si>
-  <si>
     <t>OPQA-391||OPQA-1842</t>
   </si>
   <si>
@@ -487,6 +481,30 @@
   </si>
   <si>
     <t>Verify that system should remove any leading or trailing spaces of an email address entered by the user before validating it.</t>
+  </si>
+  <si>
+    <t>OPQA-350||OPQA-2333||OPQA-1930</t>
+  </si>
+  <si>
+    <t>Verify that existing FB user is able to login and logout successfully||Verify that neon should check whether there are any other existing Neon identity with same email id and social account,if the Neon identity does not exists with STeAM account,after signing into Facebook on Neon as first user.||Verify that user can able to Sign out from Neon after successful login in "Sign In with Facebook" in Neon</t>
+  </si>
+  <si>
+    <t>IAM036</t>
+  </si>
+  <si>
+    <t>OPQA-2298</t>
+  </si>
+  <si>
+    <t>Verify that after successful registration on the NEON landing screen using Facebook, user who already has LinkedIn account with the same emailId are prompted to link their Linked account with the newly created Facebook account</t>
+  </si>
+  <si>
+    <t>IAM037</t>
+  </si>
+  <si>
+    <t>OPQA-1936</t>
+  </si>
+  <si>
+    <t>Verify that user is able to reset STeAM Password from the Neon landing page.Prerequisites: A Neon identity with a linked STeAM account.</t>
   </si>
 </sst>
 </file>
@@ -902,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -985,15 +1003,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -1007,10 +1025,10 @@
         <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -1024,10 +1042,10 @@
         <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
@@ -1075,10 +1093,10 @@
         <v>64</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>3</v>
@@ -1092,10 +1110,10 @@
         <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1126,10 +1144,10 @@
         <v>67</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1146,7 +1164,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1194,10 +1212,10 @@
         <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1510,18 +1528,52 @@
     </row>
     <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>150</v>
-      </c>
       <c r="D36" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.2">
+      <c r="A37" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8">
+      <c r="A38" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed scripts in IAM and RCC Modules.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="161">
   <si>
     <t>TCID</t>
   </si>
@@ -508,6 +508,17 @@
   <si>
     <t>Verify that system able to resend activation mail when user doesn't activated mail and 
 already registered with Neon.||Verify that,an error message should display as "email activation",when User did'nt activate the link in that respective mail after completing the registration process in Neon.||Verify that, user can click the button to resend email verification,so that the system shall send an email verification to the correct email address,if an email verification message is not sent correctly previously.||Verify that,user should sent to Neon home page after clicking the link in the Neon verification email.</t>
+  </si>
+  <si>
+    <t>IAM038</t>
+  </si>
+  <si>
+    <t>OPQA-3937||OPQA-3939||OPQA-3940||OPQA-3941||OPQA-3942||OPQA-3944||OPQA-3946||OPQA-3947||OPQA-3950||OPQA-3945||OPQA-3943||OPQA-3938</t>
+  </si>
+  <si>
+    <t>Verify that CANCEL button is working correctly when click "Change Password" link in Account setting page||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in account setting page||Verify Password must contain at least one number is ALWAYS enforced in account setting page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in account setting page||Verify that the Password minimum length of 8 characters is ALWAYS enforced in account setting page.||Verify that error message "Incorrect password. Please try again." when enter Incorrect existing STeAM password in old password field for account setting page.|| 
+Verify that error message "New password should not match current password." when enter Old and New password are same in account setting page.||Verify that error message "New password should not match previous 4 passwords." when enter new password match with previous four passwords.||Verify that user receive a conformation mail when user changed password in account setting page.|| 
+Verify that Password rules are displaying when New STeAM password does not meet password requirements in account setting page||Verify Password Maximum Length of 95 characters is ALWAYS enforced in account setting page||Verify that "Forgot password?" link working correctly when click "Change Password" link in Account setting page and that he is able to login with his new password</t>
   </si>
 </sst>
 </file>
@@ -928,19 +939,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -960,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45">
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -977,7 +988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90">
+    <row r="3" spans="1:5" ht="86.4">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
@@ -1011,7 +1022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
@@ -1028,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -1045,7 +1056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
@@ -1062,7 +1073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="4" t="s">
         <v>61</v>
       </c>
@@ -1079,7 +1090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="4" t="s">
         <v>62</v>
       </c>
@@ -1096,7 +1107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
@@ -1113,7 +1124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="43.2">
       <c r="A11" s="11" t="s">
         <v>64</v>
       </c>
@@ -1147,7 +1158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="75">
+    <row r="13" spans="1:5" ht="57.6">
       <c r="A13" s="4" t="s">
         <v>66</v>
       </c>
@@ -1164,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
@@ -1181,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="4" t="s">
         <v>69</v>
       </c>
@@ -1198,7 +1209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="4" t="s">
         <v>70</v>
       </c>
@@ -1215,7 +1226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="90">
+    <row r="17" spans="1:5" ht="86.4">
       <c r="A17" s="4" t="s">
         <v>71</v>
       </c>
@@ -1266,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="105">
+    <row r="20" spans="1:5" ht="100.8">
       <c r="A20" s="4" t="s">
         <v>67</v>
       </c>
@@ -1283,7 +1294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>74</v>
       </c>
@@ -1317,7 +1328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="4" t="s">
         <v>76</v>
       </c>
@@ -1419,7 +1430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="150">
+    <row r="29" spans="1:5" ht="129.6">
       <c r="A29" s="4" t="s">
         <v>106</v>
       </c>
@@ -1436,7 +1447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="4" t="s">
         <v>107</v>
       </c>
@@ -1453,7 +1464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="28.8">
       <c r="A31" s="4" t="s">
         <v>110</v>
       </c>
@@ -1470,7 +1481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>111</v>
       </c>
@@ -1487,7 +1498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45">
+    <row r="33" spans="1:5" ht="43.2">
       <c r="A33" s="2" t="s">
         <v>116</v>
       </c>
@@ -1502,7 +1513,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="90">
+    <row r="34" spans="1:5" ht="86.4">
       <c r="A34" s="2" t="s">
         <v>119</v>
       </c>
@@ -1517,7 +1528,7 @@
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="150">
+    <row r="35" spans="1:5" ht="129.6">
       <c r="A35" s="14" t="s">
         <v>123</v>
       </c>
@@ -1534,7 +1545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="14" t="s">
         <v>143</v>
       </c>
@@ -1551,7 +1562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="60">
+    <row r="37" spans="1:5" ht="43.2">
       <c r="A37" s="14" t="s">
         <v>148</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30">
+    <row r="38" spans="1:5" ht="28.8">
       <c r="A38" s="14" t="s">
         <v>151</v>
       </c>
@@ -1582,6 +1593,23 @@
         <v>3</v>
       </c>
       <c r="E38" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="216">
+      <c r="A39" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1599,10 +1627,10 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1689,7 +1717,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1760,10 +1788,10 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1836,10 +1864,10 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1911,11 +1939,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2029,11 +2057,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2144,11 +2172,11 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2262,12 +2290,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2401,11 +2429,11 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2469,13 +2497,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Added removed ENWIAM017.java file and modified IAM.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -477,9 +477,6 @@
     <t>OPQA-1936</t>
   </si>
   <si>
-    <t>Verify that user is able to reset STeAM Password from the Neon landing page.Prerequisites: A Neon identity with a linked STeAM account.</t>
-  </si>
-  <si>
     <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
 8)        \
 9)        :
 10)      ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user is able to reset STeAM Password from the Neon landing page.Prerequisites: A Neon identity with a linked STeAM account. </t>
   </si>
 </sst>
 </file>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1305,7 +1305,7 @@
         <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1353,7 +1353,7 @@
         <v>73</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>46</v>
@@ -1455,10 +1455,10 @@
         <v>102</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1538,7 +1538,7 @@
         <v>115</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>116</v>
@@ -1607,7 +1607,7 @@
         <v>148</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>3</v>
@@ -1618,13 +1618,13 @@
     </row>
     <row r="39" spans="1:5" ht="216">
       <c r="A39" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="C39" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>156</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>3</v>
@@ -1643,7 +1643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added jiraid to iam.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="IAM019" sheetId="13" r:id="rId10"/>
     <sheet name="IAM029" sheetId="14" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -365,14 +365,6 @@
     <t>IAM032</t>
   </si>
   <si>
-    <t>OPQA-TBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Sign-in with Steam and link existing social account with matching email.
-2) Sign-in with Steam account which already has linked social account.
-</t>
-  </si>
-  <si>
     <t>IAM033</t>
   </si>
   <si>
@@ -475,9 +467,6 @@
   </si>
   <si>
     <t>OPQA-1936</t>
-  </si>
-  <si>
-    <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336</t>
   </si>
   <si>
     <t>OPQA-854||OPQA-853</t>
@@ -540,12 +529,24 @@
   <si>
     <t xml:space="preserve">Verify that user is able to reset STeAM Password from the Neon landing page.Prerequisites: A Neon identity with a linked STeAM account. </t>
   </si>
+  <si>
+    <t>OPQA-3879||OPQA-3881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Sign-in with Steam and link existing social account with matching email.
+2) Sign-in with Steam account which already has linked social account.
+Verify that user should never be prompted to link accounts, when sign in first time on Neon landing screen using social.||Verify that user should be prompted to link accounts, when sign in first time on Neon landing screen using STeAM. (Note:User should already been sign into social)
+</t>
+  </si>
+  <si>
+    <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336||OPQA-2273</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,6 +672,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -717,7 +726,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,9 +758,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -783,6 +793,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -958,23 +969,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.33203125" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.28515625" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,15 +1002,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1008,15 +1019,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="86.4">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1025,15 +1036,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1042,15 +1053,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="72">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -1059,15 +1070,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -1076,15 +1087,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
@@ -1093,7 +1104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
@@ -1110,7 +1121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
@@ -1127,15 +1138,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.2">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>3</v>
@@ -1144,15 +1155,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.2">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1161,7 +1172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>62</v>
       </c>
@@ -1178,15 +1189,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57.6">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1195,7 +1206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1203,7 +1214,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1212,7 +1223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
@@ -1229,7 +1240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
@@ -1246,15 +1257,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="86.4">
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1263,7 +1274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>69</v>
       </c>
@@ -1280,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>70</v>
       </c>
@@ -1297,7 +1308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="172.8">
+    <row r="20" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
@@ -1305,7 +1316,7 @@
         <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1314,7 +1325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>71</v>
       </c>
@@ -1331,7 +1342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>72</v>
       </c>
@@ -1348,12 +1359,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>46</v>
@@ -1365,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
@@ -1382,7 +1393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>76</v>
       </c>
@@ -1416,7 +1427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
@@ -1433,7 +1444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>97</v>
       </c>
@@ -1450,15 +1461,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="129.6">
+    <row r="29" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1467,7 +1478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
@@ -1484,7 +1495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>106</v>
       </c>
@@ -1501,7 +1512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
@@ -1518,46 +1529,46 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="43.2">
+    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" ht="86.4">
-      <c r="A34" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" ht="129.6">
-      <c r="A35" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="D35" s="14" t="s">
         <v>3</v>
       </c>
@@ -1565,16 +1576,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>141</v>
-      </c>
       <c r="D36" s="14" t="s">
         <v>3</v>
       </c>
@@ -1582,32 +1593,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="43.2">
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="D37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="B38" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="28.8">
-      <c r="A38" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>148</v>
-      </c>
       <c r="C38" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>3</v>
@@ -1616,15 +1627,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="216">
+    <row r="39" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>3</v>
@@ -1640,20 +1651,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1664,9 +1675,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1675,7 +1686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1686,7 +1697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1697,9 +1708,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -1708,9 +1719,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -1719,53 +1730,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -1785,16 +1796,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1808,7 +1819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -1822,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -1836,7 +1847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>93</v>
       </c>
@@ -1856,20 +1867,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1883,7 +1894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1897,7 +1908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1911,7 +1922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1932,20 +1943,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1959,7 +1970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1973,7 +1984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1987,7 +1998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2007,21 +2018,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2035,7 +2046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
@@ -2049,7 +2060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>82</v>
       </c>
@@ -2063,7 +2074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -2077,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2087,7 +2098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>84</v>
       </c>
@@ -2099,7 +2110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>83</v>
@@ -2111,7 +2122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
     </row>
   </sheetData>
@@ -2125,21 +2136,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2153,7 +2164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>87</v>
       </c>
@@ -2167,7 +2178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -2181,7 +2192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -2195,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2205,7 +2216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>84</v>
       </c>
@@ -2217,7 +2228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>83</v>
@@ -2240,21 +2251,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2268,7 +2279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>79</v>
       </c>
@@ -2282,7 +2293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>77</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -2310,7 +2321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2320,7 +2331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>79</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>78</v>
@@ -2358,22 +2369,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2393,7 +2404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>246</v>
       </c>
@@ -2411,7 +2422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>247</v>
       </c>
@@ -2429,7 +2440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>248</v>
       </c>
@@ -2449,7 +2460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -2467,7 +2478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2497,21 +2508,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2525,7 +2536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -2539,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2565,23 +2576,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
@@ -2621,7 +2632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
@@ -2641,7 +2652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -2661,7 +2672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -2681,7 +2692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Added new script in IAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="169">
   <si>
     <t>TCID</t>
   </si>
@@ -541,12 +541,21 @@
   <si>
     <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336||OPQA-2273||OPQA-3608||OPQA-1825||OPQA-1827||OPQA-1829</t>
   </si>
+  <si>
+    <t>IAM039</t>
+  </si>
+  <si>
+    <t>Verify that new window open while click on "Intellectual Property &amp; Science is now known as Clarivate Analytics, and is no longer part of Thomson Reuters" link in Neon login page.</t>
+  </si>
+  <si>
+    <t>OPQA-4500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -726,7 +735,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -758,10 +767,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,7 +801,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -969,23 +976,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.6640625" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="86.4">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -1036,7 +1043,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -1070,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" s="4" t="s">
         <v>56</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
@@ -1104,7 +1111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
@@ -1121,7 +1128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="4" t="s">
         <v>60</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.2">
       <c r="A11" s="11" t="s">
         <v>61</v>
       </c>
@@ -1172,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
         <v>62</v>
       </c>
@@ -1189,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6">
       <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
@@ -1206,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1223,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
@@ -1240,7 +1247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="86.4">
       <c r="A17" s="4" t="s">
         <v>68</v>
       </c>
@@ -1274,7 +1281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>69</v>
       </c>
@@ -1291,7 +1298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>70</v>
       </c>
@@ -1308,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="172.8">
       <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
@@ -1325,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>71</v>
       </c>
@@ -1342,7 +1349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>72</v>
       </c>
@@ -1359,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
@@ -1393,7 +1400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
@@ -1410,7 +1417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>76</v>
       </c>
@@ -1427,7 +1434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
@@ -1444,7 +1451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>97</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="129.6">
       <c r="A29" s="4" t="s">
         <v>102</v>
       </c>
@@ -1478,7 +1485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
@@ -1495,7 +1502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8">
       <c r="A31" s="4" t="s">
         <v>106</v>
       </c>
@@ -1512,7 +1519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="100.8">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -1544,7 +1551,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="86.4">
       <c r="A34" s="2" t="s">
         <v>113</v>
       </c>
@@ -1559,7 +1566,7 @@
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="129.6">
       <c r="A35" s="14" t="s">
         <v>117</v>
       </c>
@@ -1576,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="14" t="s">
         <v>137</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="43.2">
       <c r="A37" s="14" t="s">
         <v>142</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="28.8">
       <c r="A38" s="14" t="s">
         <v>145</v>
       </c>
@@ -1627,7 +1634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="330" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="216">
       <c r="A39" s="14" t="s">
         <v>150</v>
       </c>
@@ -1641,6 +1648,23 @@
         <v>3</v>
       </c>
       <c r="E39" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="43.2">
+      <c r="A40" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1651,20 +1675,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1675,7 +1699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>153</v>
       </c>
@@ -1686,7 +1710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1697,7 +1721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1708,7 +1732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>159</v>
       </c>
@@ -1719,7 +1743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>160</v>
       </c>
@@ -1730,7 +1754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>154</v>
       </c>
@@ -1741,7 +1765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>155</v>
       </c>
@@ -1752,7 +1776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>156</v>
       </c>
@@ -1763,7 +1787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
@@ -1774,7 +1798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>158</v>
       </c>
@@ -1796,16 +1820,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1819,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -1833,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -1847,7 +1871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>
@@ -1867,20 +1891,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1894,7 +1918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1908,7 +1932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1922,7 +1946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1943,20 +1967,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1970,7 +1994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1984,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1998,7 +2022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2018,21 +2042,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2046,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
@@ -2060,7 +2084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>82</v>
       </c>
@@ -2074,7 +2098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -2088,7 +2112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2098,7 +2122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>84</v>
       </c>
@@ -2110,7 +2134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>83</v>
@@ -2122,7 +2146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="10"/>
     </row>
   </sheetData>
@@ -2136,21 +2160,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2164,7 +2188,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>87</v>
       </c>
@@ -2178,7 +2202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -2192,7 +2216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -2206,7 +2230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2216,7 +2240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>84</v>
       </c>
@@ -2228,7 +2252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>83</v>
@@ -2251,21 +2275,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2279,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>79</v>
       </c>
@@ -2293,7 +2317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>77</v>
       </c>
@@ -2307,7 +2331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -2321,7 +2345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2331,7 +2355,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>79</v>
       </c>
@@ -2343,7 +2367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>78</v>
@@ -2369,22 +2393,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2404,7 +2428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="5">
         <v>246</v>
       </c>
@@ -2422,7 +2446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="5">
         <v>247</v>
       </c>
@@ -2440,7 +2464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5">
         <v>248</v>
       </c>
@@ -2460,7 +2484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -2478,7 +2502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2508,21 +2532,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2536,7 +2560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -2550,7 +2574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2576,23 +2600,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2612,7 +2636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
@@ -2632,7 +2656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
@@ -2652,7 +2676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -2672,7 +2696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -2692,7 +2716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Fixed Script in IAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -433,12 +433,6 @@
     <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly in Neon and ENW landing page</t>
   </si>
   <si>
-    <t>Verify that user is able to change his STeAM password by using Forgot Password link and that he is able to login with his new password||Verify Upon completion of establishing a new password, a user who wants to go to Neon shall be presented a confirmation page with an optional link back to Neon Landing page.||Verify that,the system should support a Neon password reset workflow with the following configurations:</t>
-  </si>
-  <si>
-    <t>OPQA-535||OPQA-1955||OPQA-3686</t>
-  </si>
-  <si>
     <t>IAM035</t>
   </si>
   <si>
@@ -549,6 +543,12 @@
   </si>
   <si>
     <t>OPQA-4500</t>
+  </si>
+  <si>
+    <t>OPQA-1934||OPQA-1935||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-4261||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
   </si>
 </sst>
 </file>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1065,10 +1065,10 @@
         <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -1264,15 +1264,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="86.4">
+    <row r="17" spans="1:5" ht="201.6">
       <c r="A17" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1323,7 +1323,7 @@
         <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1371,7 +1371,7 @@
         <v>73</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>46</v>
@@ -1473,10 +1473,10 @@
         <v>102</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1541,10 +1541,10 @@
         <v>112</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1556,7 +1556,7 @@
         <v>113</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>114</v>
@@ -1585,13 +1585,13 @@
     </row>
     <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>137</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>3</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="37" spans="1:5" ht="43.2">
       <c r="A37" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>144</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>3</v>
@@ -1619,13 +1619,13 @@
     </row>
     <row r="38" spans="1:5" ht="28.8">
       <c r="A38" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>3</v>
@@ -1636,13 +1636,13 @@
     </row>
     <row r="39" spans="1:5" ht="216">
       <c r="A39" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>3</v>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="40" spans="1:5" ht="43.2">
       <c r="A40" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>168</v>
-      </c>
       <c r="C40" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>3</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Created new scripts in IAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="175">
   <si>
     <t>TCID</t>
   </si>
@@ -548,12 +548,6 @@
     <t>IAM040</t>
   </si>
   <si>
-    <t>OPQA-5372||OPQA-5373||OPQA-4252</t>
-  </si>
-  <si>
-    <t>Verify that error message "Please enter an email address." should be displayed in red color when user not enter email address in email text field for neon login page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter email address in email text field for neon login page||Verify that error message " Please enter a valid email address." should be displayed in red color when user enters email address in wrong format</t>
-  </si>
-  <si>
     <t>OPQA-1934||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||
 OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
   </si>
@@ -561,6 +555,21 @@
     <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||
 Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||
 Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp; Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
+  </si>
+  <si>
+    <t>OPQA-5372||OPQA-5373||OPQA-4252||OPQA-5401||OPQA-5402</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter a valid email address." should be displayed in red color when user not enter email address in email text field for neon login page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter password in password text field for neon login page||Verify that error message " Please enter a valid email address." should be displayed in red color when user enters email address in wrong format||Verify that error messages "Please enter a valid email address." and "Please enter a password." should be displayed in red color when user click login button without enter username and password.||Verify that error message "Invalid email/password. Please try again." should be displayed in red color when user entered wrong username and password in login page.</t>
+  </si>
+  <si>
+    <t>IAM041</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter an email address." should be displayed in red color when user not enter email address in email text field for neon singup page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter password in password text field for neon singup page.||Verify that error message "Please enter your first name." should be displayed in red color when user not enter first name in first name text field for neon singup page.||Verify that error message "Please enter your last name." should be displayed in red color when user not enter last name in last name text field for neon singup page.</t>
+  </si>
+  <si>
+    <t>OPQA-5403||OPQA-5404||OPQA-5405||OPQA-5406</t>
   </si>
 </sst>
 </file>
@@ -989,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1281,10 +1290,10 @@
         <v>68</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1680,20 +1689,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="86.4">
+    <row r="41" spans="1:5" ht="158.4">
       <c r="A41" s="14" t="s">
         <v>167</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="129.6">
+      <c r="A42" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2308,7 +2334,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added New forgot password page Script in IAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -542,34 +542,34 @@
     <t>IAM040</t>
   </si>
   <si>
-    <t>OPQA-1934||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||
+    <t>OPQA-5372||OPQA-5373||OPQA-4252||OPQA-5401||OPQA-5402</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter a valid email address." should be displayed in red color when user not enter email address in email text field for neon login page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter password in password text field for neon login page||Verify that error message " Please enter a valid email address." should be displayed in red color when user enters email address in wrong format||Verify that error messages "Please enter a valid email address." and "Please enter a password." should be displayed in red color when user click login button without enter username and password.||Verify that error message "Invalid email/password. Please try again." should be displayed in red color when user entered wrong username and password in login page.</t>
+  </si>
+  <si>
+    <t>IAM041</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter an email address." should be displayed in red color when user not enter email address in email text field for neon singup page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter password in password text field for neon singup page.||Verify that error message "Please enter your first name." should be displayed in red color when user not enter first name in first name text field for neon singup page.||Verify that error message "Please enter your last name." should be displayed in red color when user not enter last name in last name text field for neon singup page.</t>
+  </si>
+  <si>
+    <t>OPQA-5403||OPQA-5404||OPQA-5405||OPQA-5406</t>
+  </si>
+  <si>
+    <t>OPQA-527&amp;&amp;OPQA-5415</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.&amp;&amp;Verify that Last sign in time should be displayed in account setting page</t>
+  </si>
+  <si>
+    <t>OPQA-1934||OPQA-5207&amp;&amp;OPQA-5138||OPQA-5208||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-5133||
 OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
   </si>
   <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters is replaced with Clarivate Analytics to all neon pages related forgot password&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify that the Project Neon should be displayed on the forgot password page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'Project Neon' should be moved within the white area and should be above 'Reset your Password' text and center aligned||
 Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||
 Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp; Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
-  </si>
-  <si>
-    <t>OPQA-5372||OPQA-5373||OPQA-4252||OPQA-5401||OPQA-5402</t>
-  </si>
-  <si>
-    <t>Verify that error message "Please enter a valid email address." should be displayed in red color when user not enter email address in email text field for neon login page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter password in password text field for neon login page||Verify that error message " Please enter a valid email address." should be displayed in red color when user enters email address in wrong format||Verify that error messages "Please enter a valid email address." and "Please enter a password." should be displayed in red color when user click login button without enter username and password.||Verify that error message "Invalid email/password. Please try again." should be displayed in red color when user entered wrong username and password in login page.</t>
-  </si>
-  <si>
-    <t>IAM041</t>
-  </si>
-  <si>
-    <t>Verify that error message "Please enter an email address." should be displayed in red color when user not enter email address in email text field for neon singup page.||Verify that error message "Please enter a password." should be displayed in red color when user not enter password in password text field for neon singup page.||Verify that error message "Please enter your first name." should be displayed in red color when user not enter first name in first name text field for neon singup page.||Verify that error message "Please enter your last name." should be displayed in red color when user not enter last name in last name text field for neon singup page.</t>
-  </si>
-  <si>
-    <t>OPQA-5403||OPQA-5404||OPQA-5405||OPQA-5406</t>
-  </si>
-  <si>
-    <t>OPQA-527&amp;&amp;OPQA-5415</t>
-  </si>
-  <si>
-    <t>Verify change password link in the account page is working correctly.&amp;&amp;Verify that Last sign in time should be displayed in account setting page</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1290,10 +1290,10 @@
         <v>66</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1409,10 +1409,10 @@
         <v>72</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1694,10 +1694,10 @@
         <v>165</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>3</v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="42" spans="1:5" ht="129.6">
       <c r="A42" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="17" t="s">
-        <v>172</v>
-      </c>
       <c r="C42" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Removed sleep method in IAM Module scripts.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IAM.xlsx
+++ b/src/test/resources/xls/IAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -552,8 +552,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,7 +733,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -765,10 +765,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,7 +799,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -976,23 +974,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.6640625" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -1026,7 +1024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="86.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -1043,7 +1041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1060,7 +1058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -1077,7 +1075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -1094,7 +1092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1111,7 +1109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="4" t="s">
         <v>56</v>
       </c>
@@ -1128,7 +1126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
@@ -1145,7 +1143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="4" t="s">
         <v>58</v>
       </c>
@@ -1162,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.2">
       <c r="A11" s="11" t="s">
         <v>59</v>
       </c>
@@ -1179,7 +1177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
         <v>60</v>
       </c>
@@ -1196,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6">
       <c r="A13" s="4" t="s">
         <v>61</v>
       </c>
@@ -1213,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -1230,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
@@ -1247,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -1264,7 +1262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="230.4">
       <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
@@ -1281,7 +1279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>67</v>
       </c>
@@ -1298,7 +1296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>68</v>
       </c>
@@ -1315,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="172.8">
       <c r="A20" s="4" t="s">
         <v>62</v>
       </c>
@@ -1332,7 +1330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>69</v>
       </c>
@@ -1349,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>70</v>
       </c>
@@ -1366,7 +1364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="4" t="s">
         <v>71</v>
       </c>
@@ -1383,7 +1381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
@@ -1400,7 +1398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>73</v>
       </c>
@@ -1417,7 +1415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>74</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>94</v>
       </c>
@@ -1451,7 +1449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>95</v>
       </c>
@@ -1468,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="129.6">
       <c r="A29" s="4" t="s">
         <v>100</v>
       </c>
@@ -1485,7 +1483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="4" t="s">
         <v>101</v>
       </c>
@@ -1502,7 +1500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8">
       <c r="A31" s="4" t="s">
         <v>104</v>
       </c>
@@ -1519,7 +1517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>105</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="129.6">
       <c r="A33" s="14" t="s">
         <v>111</v>
       </c>
@@ -1553,7 +1551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="28.8">
       <c r="A34" s="14" t="s">
         <v>129</v>
       </c>
@@ -1570,7 +1568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="43.2">
       <c r="A35" s="14" t="s">
         <v>134</v>
       </c>
@@ -1587,7 +1585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="14" t="s">
         <v>137</v>
       </c>
@@ -1604,7 +1602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="330" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="216">
       <c r="A37" s="14" t="s">
         <v>142</v>
       </c>
@@ -1621,7 +1619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="43.2">
       <c r="A38" s="14" t="s">
         <v>154</v>
       </c>
@@ -1632,13 +1630,13 @@
         <v>155</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="158.4">
       <c r="A39" s="14" t="s">
         <v>159</v>
       </c>
@@ -1655,7 +1653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="129.6">
       <c r="A40" s="14" t="s">
         <v>162</v>
       </c>
@@ -1679,20 +1677,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1703,7 +1701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>144</v>
       </c>
@@ -1714,7 +1712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1725,7 +1723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1736,7 +1734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>150</v>
       </c>
@@ -1747,7 +1745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>151</v>
       </c>
@@ -1758,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
@@ -1769,7 +1767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>146</v>
       </c>
@@ -1780,7 +1778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>147</v>
       </c>
@@ -1791,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>148</v>
       </c>
@@ -1802,7 +1800,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>149</v>
       </c>
@@ -1824,16 +1822,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1847,7 +1845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -1861,7 +1859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -1875,7 +1873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>
@@ -1895,20 +1893,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1922,7 +1920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1936,7 +1934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1950,7 +1948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1971,20 +1969,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +1996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2012,7 +2010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2026,7 +2024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2046,21 +2044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2074,7 +2072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>82</v>
       </c>
@@ -2088,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>80</v>
       </c>
@@ -2102,7 +2100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>78</v>
       </c>
@@ -2116,7 +2114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2126,7 +2124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>82</v>
       </c>
@@ -2138,7 +2136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
@@ -2150,7 +2148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="10"/>
     </row>
   </sheetData>
@@ -2164,21 +2162,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2192,7 +2190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>85</v>
       </c>
@@ -2206,7 +2204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>84</v>
       </c>
@@ -2220,7 +2218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>78</v>
       </c>
@@ -2234,7 +2232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2244,7 +2242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>82</v>
       </c>
@@ -2256,7 +2254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
@@ -2279,21 +2277,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2307,7 +2305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>77</v>
       </c>
@@ -2321,7 +2319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>78</v>
       </c>
@@ -2349,7 +2347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2359,7 +2357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>77</v>
       </c>
@@ -2371,7 +2369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>76</v>
@@ -2397,22 +2395,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2432,7 +2430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="5">
         <v>246</v>
       </c>
@@ -2450,7 +2448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="5">
         <v>247</v>
       </c>
@@ -2468,7 +2466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5">
         <v>248</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -2506,7 +2504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2536,21 +2534,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2564,7 +2562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -2578,7 +2576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2604,23 +2602,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -2660,7 +2658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -2680,7 +2678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>88</v>
       </c>
@@ -2700,7 +2698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>89</v>
       </c>
@@ -2720,7 +2718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>76</v>
       </c>

</xml_diff>